<commit_message>
fix: sysco post processing
</commit_message>
<xml_diff>
--- a/analysis_docs/sysco/sysco_parsed_with_confidence.xlsx
+++ b/analysis_docs/sysco/sysco_parsed_with_confidence.xlsx
@@ -1229,10 +1229,8 @@
       <c r="C6" t="n">
         <v>0</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="D6" t="n">
+        <v>652144509</v>
       </c>
       <c r="E6" t="n">
         <v>0.96</v>
@@ -1260,10 +1258,8 @@
       <c r="L6" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>756346</t>
-        </is>
+      <c r="M6" t="n">
+        <v>756346</v>
       </c>
       <c r="N6" t="n">
         <v>0.96</v>
@@ -1561,7 +1557,7 @@
         <v>139667</v>
       </c>
       <c r="C2" t="n">
-        <v>0.975</v>
+        <v>0.972</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1592,7 +1588,7 @@
         <v>7.39</v>
       </c>
       <c r="L2" t="n">
-        <v>0.974</v>
+        <v>0.976</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -1601,7 +1597,7 @@
         <v>29.56</v>
       </c>
       <c r="O2" t="n">
-        <v>0.968</v>
+        <v>0.974</v>
       </c>
       <c r="P2" t="n">
         <v>0</v>
@@ -1659,7 +1655,7 @@
         <v>2404127</v>
       </c>
       <c r="C3" t="n">
-        <v>0.977</v>
+        <v>0.976</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -1690,7 +1686,7 @@
         <v>21.95</v>
       </c>
       <c r="L3" t="n">
-        <v>0.979</v>
+        <v>0.981</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -1710,7 +1706,7 @@
         </is>
       </c>
       <c r="R3" t="n">
-        <v>0.931</v>
+        <v>0.978</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
@@ -1761,7 +1757,7 @@
         <v>2441285</v>
       </c>
       <c r="C4" t="n">
-        <v>0.974</v>
+        <v>0.97</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1772,7 +1768,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.897</v>
+        <v>0.896</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -1797,7 +1793,7 @@
         <v>10.99</v>
       </c>
       <c r="O4" t="n">
-        <v>0.969</v>
+        <v>0.968</v>
       </c>
       <c r="P4" t="n">
         <v>0</v>
@@ -1808,7 +1804,7 @@
         </is>
       </c>
       <c r="R4" t="n">
-        <v>0.978</v>
+        <v>0.98</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
@@ -1826,7 +1822,7 @@
         </is>
       </c>
       <c r="X4" t="n">
-        <v>0.981</v>
+        <v>0.983</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
@@ -1835,7 +1831,7 @@
         <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.981</v>
+        <v>0.982</v>
       </c>
       <c r="AB4" t="n">
         <v>0</v>
@@ -1863,7 +1859,7 @@
         <v>2986038</v>
       </c>
       <c r="C5" t="n">
-        <v>0.975</v>
+        <v>0.972</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -1874,7 +1870,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.909</v>
+        <v>0.896</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -1890,7 +1886,7 @@
         <v>41.79</v>
       </c>
       <c r="L5" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1899,7 +1895,7 @@
         <v>41.79</v>
       </c>
       <c r="O5" t="n">
-        <v>0.969</v>
+        <v>0.973</v>
       </c>
       <c r="P5" t="n">
         <v>0</v>
@@ -1910,7 +1906,7 @@
         </is>
       </c>
       <c r="R5" t="n">
-        <v>0.909</v>
+        <v>0.925</v>
       </c>
       <c r="S5" t="n">
         <v>0</v>
@@ -1937,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.975</v>
+        <v>0.976</v>
       </c>
       <c r="AB5" t="n">
         <v>0</v>
@@ -1965,7 +1961,7 @@
         <v>7192671</v>
       </c>
       <c r="C6" t="n">
-        <v>0.972</v>
+        <v>0.971</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1976,7 +1972,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.914</v>
+        <v>0.913</v>
       </c>
       <c r="G6" t="n">
         <v>0</v>
@@ -1992,7 +1988,7 @@
         <v>28.29</v>
       </c>
       <c r="L6" t="n">
-        <v>0.97</v>
+        <v>0.975</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
@@ -2001,7 +1997,7 @@
         <v>28.29</v>
       </c>
       <c r="O6" t="n">
-        <v>0.968</v>
+        <v>0.971</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
@@ -2012,7 +2008,7 @@
         </is>
       </c>
       <c r="R6" t="n">
-        <v>0.8110000000000001</v>
+        <v>0.891</v>
       </c>
       <c r="S6" t="n">
         <v>0</v>
@@ -2030,7 +2026,7 @@
         </is>
       </c>
       <c r="X6" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="Y6" t="n">
         <v>0</v>
@@ -2039,7 +2035,7 @@
         <v>1</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.978</v>
+        <v>0.98</v>
       </c>
       <c r="AB6" t="n">
         <v>0</v>
@@ -2067,7 +2063,7 @@
         <v>3601598</v>
       </c>
       <c r="C7" t="n">
-        <v>0.969</v>
+        <v>0.967</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -2078,7 +2074,7 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0.896</v>
+        <v>0.895</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -2094,7 +2090,7 @@
         <v>111.95</v>
       </c>
       <c r="L7" t="n">
-        <v>0.977</v>
+        <v>0.975</v>
       </c>
       <c r="M7" t="n">
         <v>0</v>
@@ -2103,7 +2099,7 @@
         <v>111.95</v>
       </c>
       <c r="O7" t="n">
-        <v>0.961</v>
+        <v>0.965</v>
       </c>
       <c r="P7" t="n">
         <v>0</v>
@@ -2114,7 +2110,7 @@
         </is>
       </c>
       <c r="R7" t="n">
-        <v>0.914</v>
+        <v>0.9</v>
       </c>
       <c r="S7" t="n">
         <v>0</v>
@@ -2132,7 +2128,7 @@
         </is>
       </c>
       <c r="X7" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="Y7" t="n">
         <v>0</v>
@@ -2141,7 +2137,7 @@
         <v>1</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.968</v>
+        <v>0.974</v>
       </c>
       <c r="AB7" t="n">
         <v>0</v>
@@ -2169,7 +2165,7 @@
         <v>7757966</v>
       </c>
       <c r="C8" t="n">
-        <v>0.972</v>
+        <v>0.967</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -2180,7 +2176,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0.877</v>
+        <v>0.89</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -2205,7 +2201,7 @@
         <v>113.99</v>
       </c>
       <c r="O8" t="n">
-        <v>0.961</v>
+        <v>0.967</v>
       </c>
       <c r="P8" t="n">
         <v>0</v>
@@ -2216,7 +2212,7 @@
         </is>
       </c>
       <c r="R8" t="n">
-        <v>0.896</v>
+        <v>0.914</v>
       </c>
       <c r="S8" t="n">
         <v>0</v>
@@ -2234,7 +2230,7 @@
         </is>
       </c>
       <c r="X8" t="n">
-        <v>0.979</v>
+        <v>0.977</v>
       </c>
       <c r="Y8" t="n">
         <v>0</v>
@@ -2243,7 +2239,7 @@
         <v>1</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.971</v>
+        <v>0.974</v>
       </c>
       <c r="AB8" t="n">
         <v>0</v>
@@ -2271,7 +2267,7 @@
         <v>593606</v>
       </c>
       <c r="C9" t="n">
-        <v>0.974</v>
+        <v>0.97</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2282,7 +2278,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.893</v>
+        <v>0.894</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -2298,7 +2294,7 @@
         <v>75.48</v>
       </c>
       <c r="L9" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M9" t="n">
         <v>0</v>
@@ -2307,7 +2303,7 @@
         <v>75.48</v>
       </c>
       <c r="O9" t="n">
-        <v>0.969</v>
+        <v>0.972</v>
       </c>
       <c r="P9" t="n">
         <v>0</v>
@@ -2318,7 +2314,7 @@
         </is>
       </c>
       <c r="R9" t="n">
-        <v>0.973</v>
+        <v>0.972</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -2336,7 +2332,7 @@
         </is>
       </c>
       <c r="X9" t="n">
-        <v>0.977</v>
+        <v>0.981</v>
       </c>
       <c r="Y9" t="n">
         <v>0</v>
@@ -2345,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.974</v>
+        <v>0.975</v>
       </c>
       <c r="AB9" t="n">
         <v>0</v>
@@ -2373,7 +2369,7 @@
         <v>3909173</v>
       </c>
       <c r="C10" t="n">
-        <v>0.95</v>
+        <v>0.949</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -2384,7 +2380,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>0.877</v>
+        <v>0.889</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
@@ -2400,7 +2396,7 @@
         <v>91.84999999999999</v>
       </c>
       <c r="L10" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -2409,7 +2405,7 @@
         <v>91.84999999999999</v>
       </c>
       <c r="O10" t="n">
-        <v>0.914</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="P10" t="n">
         <v>0</v>
@@ -2420,7 +2416,7 @@
         </is>
       </c>
       <c r="R10" t="n">
-        <v>0.966</v>
+        <v>0.968</v>
       </c>
       <c r="S10" t="n">
         <v>0</v>
@@ -2447,7 +2443,7 @@
         <v>1</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.969</v>
+        <v>0.974</v>
       </c>
       <c r="AB10" t="n">
         <v>0</v>
@@ -2475,7 +2471,7 @@
         <v>7000181</v>
       </c>
       <c r="C11" t="n">
-        <v>0.971</v>
+        <v>0.967</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -2502,7 +2498,7 @@
         <v>54.95</v>
       </c>
       <c r="L11" t="n">
-        <v>0.975</v>
+        <v>0.976</v>
       </c>
       <c r="M11" t="n">
         <v>0</v>
@@ -2511,7 +2507,7 @@
         <v>109.9</v>
       </c>
       <c r="O11" t="n">
-        <v>0.968</v>
+        <v>0.957</v>
       </c>
       <c r="P11" t="n">
         <v>0</v>
@@ -2522,7 +2518,7 @@
         </is>
       </c>
       <c r="R11" t="n">
-        <v>0.947</v>
+        <v>0.948</v>
       </c>
       <c r="S11" t="n">
         <v>0</v>
@@ -2549,7 +2545,7 @@
         <v>2</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.969</v>
+        <v>0.971</v>
       </c>
       <c r="AB11" t="n">
         <v>0</v>
@@ -2604,7 +2600,7 @@
         <v>78.95</v>
       </c>
       <c r="L12" t="n">
-        <v>0.976</v>
+        <v>0.977</v>
       </c>
       <c r="M12" t="n">
         <v>0</v>
@@ -2613,7 +2609,7 @@
         <v>78.95</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.951</v>
       </c>
       <c r="P12" t="n">
         <v>0</v>
@@ -2642,7 +2638,7 @@
         </is>
       </c>
       <c r="X12" t="n">
-        <v>0.977</v>
+        <v>0.981</v>
       </c>
       <c r="Y12" t="n">
         <v>0</v>
@@ -2651,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.976</v>
+        <v>0.975</v>
       </c>
       <c r="AB12" t="n">
         <v>0</v>
@@ -2679,7 +2675,7 @@
         <v>106664</v>
       </c>
       <c r="C13" t="n">
-        <v>0.97</v>
+        <v>0.972</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -2690,7 +2686,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0.902</v>
+        <v>0.914</v>
       </c>
       <c r="G13" t="n">
         <v>0</v>
@@ -2710,7 +2706,7 @@
         <v>65.25</v>
       </c>
       <c r="L13" t="n">
-        <v>0.975</v>
+        <v>0.976</v>
       </c>
       <c r="M13" t="n">
         <v>0</v>
@@ -2719,18 +2715,18 @@
         <v>65.25</v>
       </c>
       <c r="O13" t="n">
+        <v>0.956</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>LB</t>
+        </is>
+      </c>
+      <c r="R13" t="n">
         <v>0.973</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>LB</t>
-        </is>
-      </c>
-      <c r="R13" t="n">
-        <v>0.977</v>
       </c>
       <c r="S13" t="n">
         <v>0</v>
@@ -2748,7 +2744,7 @@
         </is>
       </c>
       <c r="X13" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="Y13" t="n">
         <v>0</v>
@@ -2757,7 +2753,7 @@
         <v>1</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.978</v>
+        <v>0.964</v>
       </c>
       <c r="AB13" t="n">
         <v>0</v>
@@ -2785,7 +2781,7 @@
         <v>3011295</v>
       </c>
       <c r="C14" t="n">
-        <v>0.972</v>
+        <v>0.967</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -2796,7 +2792,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>0.901</v>
+        <v>0.911</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
@@ -2825,7 +2821,7 @@
         <v>60.85</v>
       </c>
       <c r="O14" t="n">
-        <v>0.972</v>
+        <v>0.967</v>
       </c>
       <c r="P14" t="n">
         <v>0</v>
@@ -2836,7 +2832,7 @@
         </is>
       </c>
       <c r="R14" t="n">
-        <v>0.972</v>
+        <v>0.98</v>
       </c>
       <c r="S14" t="n">
         <v>0</v>
@@ -2863,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.976</v>
+        <v>0.969</v>
       </c>
       <c r="AB14" t="n">
         <v>0</v>
@@ -2891,7 +2887,7 @@
         <v>7040473</v>
       </c>
       <c r="C15" t="n">
-        <v>0.973</v>
+        <v>0.969</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -2902,7 +2898,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>0.896</v>
+        <v>0.9340000000000001</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
@@ -2927,7 +2923,7 @@
         <v>68.79000000000001</v>
       </c>
       <c r="O15" t="n">
-        <v>0.97</v>
+        <v>0.967</v>
       </c>
       <c r="P15" t="n">
         <v>0</v>
@@ -2938,7 +2934,7 @@
         </is>
       </c>
       <c r="R15" t="n">
-        <v>0.755</v>
+        <v>0.819</v>
       </c>
       <c r="S15" t="n">
         <v>0</v>
@@ -2965,7 +2961,7 @@
         <v>1</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.972</v>
+        <v>0.973</v>
       </c>
       <c r="AB15" t="n">
         <v>0</v>
@@ -2993,7 +2989,7 @@
         <v>4518403</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9419999999999999</v>
+        <v>0.971</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -3004,7 +3000,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0.923</v>
+        <v>0.9389999999999999</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
@@ -3020,7 +3016,7 @@
         <v>35.65</v>
       </c>
       <c r="L16" t="n">
-        <v>0.966</v>
+        <v>0.978</v>
       </c>
       <c r="M16" t="n">
         <v>0</v>
@@ -3029,7 +3025,7 @@
         <v>35.65</v>
       </c>
       <c r="O16" t="n">
-        <v>0.914</v>
+        <v>0.968</v>
       </c>
       <c r="P16" t="n">
         <v>0</v>
@@ -3040,7 +3036,7 @@
         </is>
       </c>
       <c r="R16" t="n">
-        <v>0.964</v>
+        <v>0.974</v>
       </c>
       <c r="S16" t="n">
         <v>0</v>
@@ -3058,7 +3054,7 @@
         </is>
       </c>
       <c r="X16" t="n">
-        <v>0.979</v>
+        <v>0.981</v>
       </c>
       <c r="Y16" t="n">
         <v>0</v>
@@ -3067,7 +3063,7 @@
         <v>1</v>
       </c>
       <c r="AA16" t="n">
-        <v>0.983</v>
+        <v>0.984</v>
       </c>
       <c r="AB16" t="n">
         <v>0</v>
@@ -3095,7 +3091,7 @@
         <v>5229125</v>
       </c>
       <c r="C17" t="n">
-        <v>0.972</v>
+        <v>0.969</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -3106,7 +3102,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>0.853</v>
+        <v>0.866</v>
       </c>
       <c r="G17" t="n">
         <v>0</v>
@@ -3135,7 +3131,7 @@
         <v>15.15</v>
       </c>
       <c r="O17" t="n">
-        <v>0.972</v>
+        <v>0.969</v>
       </c>
       <c r="P17" t="n">
         <v>0</v>
@@ -3146,7 +3142,7 @@
         </is>
       </c>
       <c r="R17" t="n">
-        <v>0.349</v>
+        <v>0.355</v>
       </c>
       <c r="S17" t="n">
         <v>0</v>
@@ -3197,7 +3193,7 @@
         <v>5602891</v>
       </c>
       <c r="C18" t="n">
-        <v>0.974</v>
+        <v>0.972</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -3208,7 +3204,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>0.923</v>
+        <v>0.926</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
@@ -3233,7 +3229,7 @@
         <v>96.75</v>
       </c>
       <c r="O18" t="n">
-        <v>0.972</v>
+        <v>0.971</v>
       </c>
       <c r="P18" t="n">
         <v>0</v>
@@ -3244,7 +3240,7 @@
         </is>
       </c>
       <c r="R18" t="n">
-        <v>0.962</v>
+        <v>0.946</v>
       </c>
       <c r="S18" t="n">
         <v>0</v>
@@ -3271,7 +3267,7 @@
         <v>1</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.974</v>
+        <v>0.975</v>
       </c>
       <c r="AB18" t="n">
         <v>0</v>
@@ -3299,7 +3295,7 @@
         <v>952018</v>
       </c>
       <c r="C19" t="n">
-        <v>0.974</v>
+        <v>0.976</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -3310,7 +3306,7 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>0.914</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
@@ -3326,7 +3322,7 @@
         <v>49.25</v>
       </c>
       <c r="L19" t="n">
-        <v>0.978</v>
+        <v>0.977</v>
       </c>
       <c r="M19" t="n">
         <v>0</v>
@@ -3335,7 +3331,7 @@
         <v>49.25</v>
       </c>
       <c r="O19" t="n">
-        <v>0.962</v>
+        <v>0.965</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
@@ -3369,7 +3365,7 @@
         <v>1</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.981</v>
+        <v>0.977</v>
       </c>
       <c r="AB19" t="n">
         <v>0</v>
@@ -3397,7 +3393,7 @@
         <v>1099589</v>
       </c>
       <c r="C20" t="n">
-        <v>0.946</v>
+        <v>0.95</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -3408,7 +3404,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>0.867</v>
+        <v>0.894</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
@@ -3424,7 +3420,7 @@
         <v>15.65</v>
       </c>
       <c r="L20" t="n">
-        <v>0.961</v>
+        <v>0.967</v>
       </c>
       <c r="M20" t="n">
         <v>0</v>
@@ -3433,7 +3429,7 @@
         <v>31.3</v>
       </c>
       <c r="O20" t="n">
-        <v>0.896</v>
+        <v>0.911</v>
       </c>
       <c r="P20" t="n">
         <v>0</v>
@@ -3444,7 +3440,7 @@
         </is>
       </c>
       <c r="R20" t="n">
-        <v>0.946</v>
+        <v>0.944</v>
       </c>
       <c r="S20" t="n">
         <v>0</v>
@@ -3462,7 +3458,7 @@
         </is>
       </c>
       <c r="X20" t="n">
-        <v>0.975</v>
+        <v>0.977</v>
       </c>
       <c r="Y20" t="n">
         <v>0</v>
@@ -3499,7 +3495,7 @@
         <v>1985274</v>
       </c>
       <c r="C21" t="n">
-        <v>0.969</v>
+        <v>0.967</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -3510,7 +3506,7 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.896</v>
+        <v>0.889</v>
       </c>
       <c r="G21" t="n">
         <v>0</v>
@@ -3530,7 +3526,7 @@
         <v>11.29</v>
       </c>
       <c r="L21" t="n">
-        <v>0.97</v>
+        <v>0.976</v>
       </c>
       <c r="M21" t="n">
         <v>0</v>
@@ -3539,7 +3535,7 @@
         <v>11.29</v>
       </c>
       <c r="O21" t="n">
-        <v>0.914</v>
+        <v>0.945</v>
       </c>
       <c r="P21" t="n">
         <v>0</v>
@@ -3608,7 +3604,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.823</v>
+        <v>0.839</v>
       </c>
       <c r="G22" t="n">
         <v>0</v>
@@ -3628,7 +3624,7 @@
         <v>9.65</v>
       </c>
       <c r="L22" t="n">
-        <v>0.969</v>
+        <v>0.975</v>
       </c>
       <c r="M22" t="n">
         <v>0</v>
@@ -3637,7 +3633,7 @@
         <v>9.65</v>
       </c>
       <c r="O22" t="n">
-        <v>0.9389999999999999</v>
+        <v>0.9370000000000001</v>
       </c>
       <c r="P22" t="n">
         <v>0</v>
@@ -3648,7 +3644,7 @@
         </is>
       </c>
       <c r="R22" t="n">
-        <v>0.186</v>
+        <v>0.197</v>
       </c>
       <c r="S22" t="n">
         <v>0</v>
@@ -3699,7 +3695,7 @@
         <v>7350788</v>
       </c>
       <c r="C23" t="n">
-        <v>0.967</v>
+        <v>0.972</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -3710,7 +3706,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.895</v>
+        <v>0.889</v>
       </c>
       <c r="G23" t="n">
         <v>0</v>
@@ -3730,7 +3726,7 @@
         <v>6.89</v>
       </c>
       <c r="L23" t="n">
-        <v>0.968</v>
+        <v>0.974</v>
       </c>
       <c r="M23" t="n">
         <v>0</v>
@@ -3739,7 +3735,7 @@
         <v>6.89</v>
       </c>
       <c r="O23" t="n">
-        <v>0.96</v>
+        <v>0.967</v>
       </c>
       <c r="P23" t="n">
         <v>0</v>
@@ -3750,7 +3746,7 @@
         </is>
       </c>
       <c r="R23" t="n">
-        <v>0.888</v>
+        <v>0.896</v>
       </c>
       <c r="S23" t="n">
         <v>0</v>
@@ -3801,7 +3797,7 @@
         <v>5134376</v>
       </c>
       <c r="C24" t="n">
-        <v>0.976</v>
+        <v>0.973</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -3812,7 +3808,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.474</v>
+        <v>0.476</v>
       </c>
       <c r="G24" t="n">
         <v>0</v>
@@ -3832,7 +3828,7 @@
         <v>95.55</v>
       </c>
       <c r="L24" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M24" t="n">
         <v>0</v>
@@ -3841,7 +3837,7 @@
         <v>95.55</v>
       </c>
       <c r="O24" t="n">
-        <v>0.975</v>
+        <v>0.972</v>
       </c>
       <c r="P24" t="n">
         <v>0</v>
@@ -3852,7 +3848,7 @@
         </is>
       </c>
       <c r="R24" t="n">
-        <v>0.975</v>
+        <v>0.977</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
@@ -3870,7 +3866,7 @@
         </is>
       </c>
       <c r="X24" t="n">
-        <v>0.979</v>
+        <v>0.981</v>
       </c>
       <c r="Y24" t="n">
         <v>0</v>
@@ -3907,7 +3903,7 @@
         <v>7056141</v>
       </c>
       <c r="C25" t="n">
-        <v>0.977</v>
+        <v>0.974</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
@@ -3918,7 +3914,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.949</v>
+        <v>0.945</v>
       </c>
       <c r="G25" t="n">
         <v>0</v>
@@ -3943,7 +3939,7 @@
         <v>45.59</v>
       </c>
       <c r="O25" t="n">
-        <v>0.976</v>
+        <v>0.973</v>
       </c>
       <c r="P25" t="n">
         <v>0</v>
@@ -3954,7 +3950,7 @@
         </is>
       </c>
       <c r="R25" t="n">
-        <v>0.111</v>
+        <v>0.133</v>
       </c>
       <c r="S25" t="n">
         <v>0</v>
@@ -4009,7 +4005,7 @@
         <v>7182310</v>
       </c>
       <c r="C26" t="n">
-        <v>0.976</v>
+        <v>0.974</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -4020,7 +4016,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.854</v>
+        <v>0.864</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
@@ -4036,7 +4032,7 @@
         <v>44.99</v>
       </c>
       <c r="L26" t="n">
-        <v>0.977</v>
+        <v>0.979</v>
       </c>
       <c r="M26" t="n">
         <v>0</v>
@@ -4056,7 +4052,7 @@
         </is>
       </c>
       <c r="R26" t="n">
-        <v>0.961</v>
+        <v>0.972</v>
       </c>
       <c r="S26" t="n">
         <v>0</v>
@@ -4074,7 +4070,7 @@
         </is>
       </c>
       <c r="X26" t="n">
-        <v>0.981</v>
+        <v>0.983</v>
       </c>
       <c r="Y26" t="n">
         <v>0</v>
@@ -4083,7 +4079,7 @@
         <v>1</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="AB26" t="n">
         <v>0</v>
@@ -4111,7 +4107,7 @@
         <v>106664</v>
       </c>
       <c r="C27" t="n">
-        <v>0.974</v>
+        <v>0.973</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
@@ -4122,7 +4118,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0.894</v>
+        <v>0.896</v>
       </c>
       <c r="G27" t="n">
         <v>0</v>
@@ -4147,7 +4143,7 @@
         <v>65.25</v>
       </c>
       <c r="O27" t="n">
-        <v>0.962</v>
+        <v>0.961</v>
       </c>
       <c r="P27" t="n">
         <v>0</v>
@@ -4158,7 +4154,7 @@
         </is>
       </c>
       <c r="R27" t="n">
-        <v>0.977</v>
+        <v>0.976</v>
       </c>
       <c r="S27" t="n">
         <v>0</v>
@@ -4176,7 +4172,7 @@
         </is>
       </c>
       <c r="X27" t="n">
-        <v>0.98</v>
+        <v>0.982</v>
       </c>
       <c r="Y27" t="n">
         <v>0</v>
@@ -4185,7 +4181,7 @@
         <v>1</v>
       </c>
       <c r="AA27" t="n">
-        <v>0.978</v>
+        <v>0.972</v>
       </c>
       <c r="AB27" t="n">
         <v>0</v>
@@ -4213,7 +4209,7 @@
         <v>2152438</v>
       </c>
       <c r="C28" t="n">
-        <v>0.974</v>
+        <v>0.971</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
@@ -4224,7 +4220,7 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>0.853</v>
+        <v>0.854</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
@@ -4249,7 +4245,7 @@
         <v>44.95</v>
       </c>
       <c r="O28" t="n">
-        <v>0.974</v>
+        <v>0.967</v>
       </c>
       <c r="P28" t="n">
         <v>0</v>
@@ -4260,7 +4256,7 @@
         </is>
       </c>
       <c r="R28" t="n">
-        <v>0.927</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="S28" t="n">
         <v>0</v>
@@ -4287,7 +4283,7 @@
         <v>1</v>
       </c>
       <c r="AA28" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
       <c r="AB28" t="n">
         <v>0</v>
@@ -4315,7 +4311,7 @@
         <v>3011295</v>
       </c>
       <c r="C29" t="n">
-        <v>0.974</v>
+        <v>0.972</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -4326,7 +4322,7 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0.852</v>
+        <v>0.853</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
@@ -4351,7 +4347,7 @@
         <v>60.85</v>
       </c>
       <c r="O29" t="n">
-        <v>0.974</v>
+        <v>0.968</v>
       </c>
       <c r="P29" t="n">
         <v>0</v>
@@ -4362,7 +4358,7 @@
         </is>
       </c>
       <c r="R29" t="n">
-        <v>0.975</v>
+        <v>0.98</v>
       </c>
       <c r="S29" t="n">
         <v>0</v>
@@ -4380,7 +4376,7 @@
         </is>
       </c>
       <c r="X29" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="Y29" t="n">
         <v>0</v>
@@ -4389,7 +4385,7 @@
         <v>1</v>
       </c>
       <c r="AA29" t="n">
-        <v>0.977</v>
+        <v>0.976</v>
       </c>
       <c r="AB29" t="n">
         <v>0</v>
@@ -4428,7 +4424,7 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>0.823</v>
+        <v>0.822</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
@@ -4448,7 +4444,7 @@
         <v>43.29</v>
       </c>
       <c r="L30" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M30" t="n">
         <v>0</v>
@@ -4457,7 +4453,7 @@
         <v>43.29</v>
       </c>
       <c r="O30" t="n">
-        <v>0.971</v>
+        <v>0.974</v>
       </c>
       <c r="P30" t="n">
         <v>0</v>
@@ -4468,7 +4464,7 @@
         </is>
       </c>
       <c r="R30" t="n">
-        <v>0.971</v>
+        <v>0.979</v>
       </c>
       <c r="S30" t="n">
         <v>0</v>
@@ -4486,7 +4482,7 @@
         </is>
       </c>
       <c r="X30" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="Y30" t="n">
         <v>0</v>
@@ -4495,7 +4491,7 @@
         <v>1</v>
       </c>
       <c r="AA30" t="n">
-        <v>0.975</v>
+        <v>0.976</v>
       </c>
       <c r="AB30" t="n">
         <v>0</v>
@@ -4523,7 +4519,7 @@
         <v>5020997</v>
       </c>
       <c r="C31" t="n">
-        <v>0.974</v>
+        <v>0.973</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
@@ -4570,7 +4566,7 @@
         </is>
       </c>
       <c r="R31" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
       <c r="S31" t="n">
         <v>0</v>
@@ -4588,7 +4584,7 @@
         </is>
       </c>
       <c r="X31" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="Y31" t="n">
         <v>0</v>
@@ -4625,7 +4621,7 @@
         <v>7008629</v>
       </c>
       <c r="C32" t="n">
-        <v>0.976</v>
+        <v>0.97</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -4636,7 +4632,7 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>0.9350000000000001</v>
+        <v>0.931</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
@@ -4661,7 +4657,7 @@
         <v>45.45</v>
       </c>
       <c r="O32" t="n">
-        <v>0.968</v>
+        <v>0.966</v>
       </c>
       <c r="P32" t="n">
         <v>0</v>
@@ -4672,7 +4668,7 @@
         </is>
       </c>
       <c r="R32" t="n">
-        <v>0.976</v>
+        <v>0.977</v>
       </c>
       <c r="S32" t="n">
         <v>0</v>
@@ -4690,7 +4686,7 @@
         </is>
       </c>
       <c r="X32" t="n">
-        <v>0.979</v>
+        <v>0.978</v>
       </c>
       <c r="Y32" t="n">
         <v>0</v>
@@ -4699,7 +4695,7 @@
         <v>1</v>
       </c>
       <c r="AA32" t="n">
-        <v>0.974</v>
+        <v>0.975</v>
       </c>
       <c r="AB32" t="n">
         <v>0</v>
@@ -4738,7 +4734,7 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0.6</v>
+        <v>0.65</v>
       </c>
       <c r="G33" t="n">
         <v>0</v>
@@ -4758,7 +4754,7 @@
         <v>46.75</v>
       </c>
       <c r="L33" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M33" t="n">
         <v>0</v>
@@ -4767,7 +4763,7 @@
         <v>46.75</v>
       </c>
       <c r="O33" t="n">
-        <v>0.975</v>
+        <v>0.969</v>
       </c>
       <c r="P33" t="n">
         <v>0</v>
@@ -4778,7 +4774,7 @@
         </is>
       </c>
       <c r="R33" t="n">
-        <v>0.978</v>
+        <v>0.969</v>
       </c>
       <c r="S33" t="n">
         <v>0</v>
@@ -4796,7 +4792,7 @@
         </is>
       </c>
       <c r="X33" t="n">
-        <v>0.979</v>
+        <v>0.978</v>
       </c>
       <c r="Y33" t="n">
         <v>0</v>
@@ -4833,7 +4829,7 @@
         <v>4518403</v>
       </c>
       <c r="C34" t="n">
-        <v>0.975</v>
+        <v>0.974</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
@@ -4844,7 +4840,7 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>0.854</v>
+        <v>0.858</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
@@ -4860,7 +4856,7 @@
         <v>35.65</v>
       </c>
       <c r="L34" t="n">
-        <v>0.977</v>
+        <v>0.979</v>
       </c>
       <c r="M34" t="n">
         <v>0</v>
@@ -4869,7 +4865,7 @@
         <v>35.65</v>
       </c>
       <c r="O34" t="n">
-        <v>0.976</v>
+        <v>0.974</v>
       </c>
       <c r="P34" t="n">
         <v>0</v>
@@ -4880,7 +4876,7 @@
         </is>
       </c>
       <c r="R34" t="n">
-        <v>0.674</v>
+        <v>0.768</v>
       </c>
       <c r="S34" t="n">
         <v>0</v>
@@ -4898,7 +4894,7 @@
         </is>
       </c>
       <c r="X34" t="n">
-        <v>0.98</v>
+        <v>0.982</v>
       </c>
       <c r="Y34" t="n">
         <v>0</v>
@@ -4907,7 +4903,7 @@
         <v>1</v>
       </c>
       <c r="AA34" t="n">
-        <v>0.983</v>
+        <v>0.984</v>
       </c>
       <c r="AB34" t="n">
         <v>0</v>
@@ -5077,7 +5073,7 @@
         <v>6235501</v>
       </c>
       <c r="C37" t="n">
-        <v>0.976</v>
+        <v>0.974</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
@@ -5088,7 +5084,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>0.9370000000000001</v>
+        <v>0.946</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
@@ -5104,7 +5100,7 @@
         <v>15.99</v>
       </c>
       <c r="L37" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M37" t="n">
         <v>0</v>
@@ -5113,7 +5109,7 @@
         <v>15.99</v>
       </c>
       <c r="O37" t="n">
-        <v>0.975</v>
+        <v>0.974</v>
       </c>
       <c r="P37" t="n">
         <v>0</v>
@@ -5124,7 +5120,7 @@
         </is>
       </c>
       <c r="R37" t="n">
-        <v>0.891</v>
+        <v>0.913</v>
       </c>
       <c r="S37" t="n">
         <v>0</v>
@@ -5142,7 +5138,7 @@
         </is>
       </c>
       <c r="X37" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="Y37" t="n">
         <v>0</v>
@@ -5151,7 +5147,7 @@
         <v>1</v>
       </c>
       <c r="AA37" t="n">
-        <v>0.974</v>
+        <v>0.976</v>
       </c>
       <c r="AB37" t="n">
         <v>0</v>
@@ -5179,7 +5175,7 @@
         <v>6359673</v>
       </c>
       <c r="C38" t="n">
-        <v>0.976</v>
+        <v>0.974</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -5190,7 +5186,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.949</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
@@ -5206,7 +5202,7 @@
         <v>31.35</v>
       </c>
       <c r="L38" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M38" t="n">
         <v>0</v>
@@ -5226,7 +5222,7 @@
         </is>
       </c>
       <c r="R38" t="n">
-        <v>0.896</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="S38" t="n">
         <v>0</v>
@@ -5281,7 +5277,7 @@
         <v>7131892</v>
       </c>
       <c r="C39" t="n">
-        <v>0.976</v>
+        <v>0.974</v>
       </c>
       <c r="D39" t="n">
         <v>0</v>
@@ -5308,7 +5304,7 @@
         <v>68.84999999999999</v>
       </c>
       <c r="L39" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M39" t="n">
         <v>0</v>
@@ -5317,7 +5313,7 @@
         <v>68.84999999999999</v>
       </c>
       <c r="O39" t="n">
-        <v>0.97</v>
+        <v>0.972</v>
       </c>
       <c r="P39" t="n">
         <v>0</v>
@@ -5328,7 +5324,7 @@
         </is>
       </c>
       <c r="R39" t="n">
-        <v>0.929</v>
+        <v>0.95</v>
       </c>
       <c r="S39" t="n">
         <v>0</v>
@@ -5346,7 +5342,7 @@
         </is>
       </c>
       <c r="X39" t="n">
-        <v>0.978</v>
+        <v>0.98</v>
       </c>
       <c r="Y39" t="n">
         <v>0</v>
@@ -5355,7 +5351,7 @@
         <v>1</v>
       </c>
       <c r="AA39" t="n">
-        <v>0.976</v>
+        <v>0.977</v>
       </c>
       <c r="AB39" t="n">
         <v>0</v>
@@ -5394,7 +5390,7 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>0.865</v>
+        <v>0.853</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
@@ -5414,7 +5410,7 @@
         <v>7.39</v>
       </c>
       <c r="L40" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="M40" t="n">
         <v>0</v>
@@ -5434,7 +5430,7 @@
         </is>
       </c>
       <c r="R40" t="n">
-        <v>0.282</v>
+        <v>0.283</v>
       </c>
       <c r="S40" t="n">
         <v>0</v>
@@ -5453,10 +5449,8 @@
       <c r="Y40" t="n">
         <v>0</v>
       </c>
-      <c r="Z40" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z40" t="n">
+        <v>2</v>
       </c>
       <c r="AA40" t="n">
         <v>0.453</v>
@@ -5487,7 +5481,7 @@
         <v>621617</v>
       </c>
       <c r="C41" t="n">
-        <v>0.976</v>
+        <v>0.975</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
@@ -5498,7 +5492,7 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0.907</v>
+        <v>0.912</v>
       </c>
       <c r="G41" t="n">
         <v>0</v>
@@ -5514,7 +5508,7 @@
         <v>36.85</v>
       </c>
       <c r="L41" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="M41" t="n">
         <v>0</v>
@@ -5523,7 +5517,7 @@
         <v>36.85</v>
       </c>
       <c r="O41" t="n">
-        <v>0.975</v>
+        <v>0.977</v>
       </c>
       <c r="P41" t="n">
         <v>0</v>
@@ -5534,7 +5528,7 @@
         </is>
       </c>
       <c r="R41" t="n">
-        <v>0.961</v>
+        <v>0.968</v>
       </c>
       <c r="S41" t="n">
         <v>0</v>
@@ -5552,18 +5546,16 @@
         </is>
       </c>
       <c r="X41" t="n">
-        <v>0.981</v>
+        <v>0.978</v>
       </c>
       <c r="Y41" t="n">
         <v>0</v>
       </c>
-      <c r="Z41" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z41" t="n">
+        <v>1</v>
       </c>
       <c r="AA41" t="n">
-        <v>0.977</v>
+        <v>0.98</v>
       </c>
       <c r="AB41" t="n">
         <v>0</v>
@@ -5591,7 +5583,7 @@
         <v>2441368</v>
       </c>
       <c r="C42" t="n">
-        <v>0.978</v>
+        <v>0.977</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
@@ -5602,7 +5594,7 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>0.913</v>
+        <v>0.923</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
@@ -5618,7 +5610,7 @@
         <v>8.550000000000001</v>
       </c>
       <c r="L42" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="M42" t="n">
         <v>0</v>
@@ -5627,7 +5619,7 @@
         <v>8.550000000000001</v>
       </c>
       <c r="O42" t="n">
-        <v>0.977</v>
+        <v>0.975</v>
       </c>
       <c r="P42" t="n">
         <v>0</v>
@@ -5638,7 +5630,7 @@
         </is>
       </c>
       <c r="R42" t="n">
-        <v>0.978</v>
+        <v>0.98</v>
       </c>
       <c r="S42" t="n">
         <v>0</v>
@@ -5656,18 +5648,16 @@
         </is>
       </c>
       <c r="X42" t="n">
-        <v>0.98</v>
+        <v>0.984</v>
       </c>
       <c r="Y42" t="n">
         <v>0</v>
       </c>
-      <c r="Z42" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z42" t="n">
+        <v>1</v>
       </c>
       <c r="AA42" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="AB42" t="n">
         <v>0</v>
@@ -5695,7 +5685,7 @@
         <v>3029404</v>
       </c>
       <c r="C43" t="n">
-        <v>0.975</v>
+        <v>0.973</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -5722,7 +5712,7 @@
         <v>98.37</v>
       </c>
       <c r="L43" t="n">
-        <v>0.977</v>
+        <v>0.979</v>
       </c>
       <c r="M43" t="n">
         <v>0</v>
@@ -5731,18 +5721,18 @@
         <v>98.37</v>
       </c>
       <c r="O43" t="n">
+        <v>0.972</v>
+      </c>
+      <c r="P43" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>53.4</t>
+        </is>
+      </c>
+      <c r="R43" t="n">
         <v>0.977</v>
-      </c>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>53.4</t>
-        </is>
-      </c>
-      <c r="R43" t="n">
-        <v>0.978</v>
       </c>
       <c r="S43" t="n">
         <v>0</v>
@@ -5760,18 +5750,16 @@
         </is>
       </c>
       <c r="X43" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="Y43" t="n">
         <v>0</v>
       </c>
-      <c r="Z43" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z43" t="n">
+        <v>1</v>
       </c>
       <c r="AA43" t="n">
-        <v>0.975</v>
+        <v>0.976</v>
       </c>
       <c r="AB43" t="n">
         <v>0</v>
@@ -5799,7 +5787,7 @@
         <v>5134376</v>
       </c>
       <c r="C44" t="n">
-        <v>0.977</v>
+        <v>0.974</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -5810,7 +5798,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>0.916</v>
+        <v>0.913</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
@@ -5850,7 +5838,7 @@
         </is>
       </c>
       <c r="R44" t="n">
-        <v>0.975</v>
+        <v>0.977</v>
       </c>
       <c r="S44" t="n">
         <v>0</v>
@@ -5868,18 +5856,16 @@
         </is>
       </c>
       <c r="X44" t="n">
-        <v>0.979</v>
+        <v>0.982</v>
       </c>
       <c r="Y44" t="n">
         <v>0</v>
       </c>
-      <c r="Z44" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z44" t="n">
+        <v>1</v>
       </c>
       <c r="AA44" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="AB44" t="n">
         <v>0</v>
@@ -5907,7 +5893,7 @@
         <v>7271683</v>
       </c>
       <c r="C45" t="n">
-        <v>0.976</v>
+        <v>0.973</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
@@ -5918,7 +5904,7 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>0.894</v>
+        <v>0.893</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
@@ -5934,7 +5920,7 @@
         <v>80.98999999999999</v>
       </c>
       <c r="L45" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M45" t="n">
         <v>0</v>
@@ -5943,7 +5929,7 @@
         <v>80.98999999999999</v>
       </c>
       <c r="O45" t="n">
-        <v>0.961</v>
+        <v>0.969</v>
       </c>
       <c r="P45" t="n">
         <v>0</v>
@@ -5954,7 +5940,7 @@
         </is>
       </c>
       <c r="R45" t="n">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
       <c r="S45" t="n">
         <v>0</v>
@@ -5977,10 +5963,8 @@
       <c r="Y45" t="n">
         <v>0</v>
       </c>
-      <c r="Z45" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z45" t="n">
+        <v>1</v>
       </c>
       <c r="AA45" t="n">
         <v>0.98</v>
@@ -6011,7 +5995,7 @@
         <v>3601598</v>
       </c>
       <c r="C46" t="n">
-        <v>0.976</v>
+        <v>0.973</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
@@ -6022,7 +6006,7 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>0.916</v>
+        <v>0.896</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
@@ -6038,7 +6022,7 @@
         <v>111.95</v>
       </c>
       <c r="L46" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M46" t="n">
         <v>0</v>
@@ -6047,7 +6031,7 @@
         <v>111.95</v>
       </c>
       <c r="O46" t="n">
-        <v>0.962</v>
+        <v>0.968</v>
       </c>
       <c r="P46" t="n">
         <v>0</v>
@@ -6081,13 +6065,11 @@
       <c r="Y46" t="n">
         <v>0</v>
       </c>
-      <c r="Z46" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z46" t="n">
+        <v>1</v>
       </c>
       <c r="AA46" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
       <c r="AB46" t="n">
         <v>0</v>
@@ -6115,7 +6097,7 @@
         <v>7000181</v>
       </c>
       <c r="C47" t="n">
-        <v>0.974</v>
+        <v>0.969</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -6126,7 +6108,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>0.902</v>
+        <v>0.905</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
@@ -6151,7 +6133,7 @@
         <v>54.95</v>
       </c>
       <c r="O47" t="n">
-        <v>0.97</v>
+        <v>0.961</v>
       </c>
       <c r="P47" t="n">
         <v>0</v>
@@ -6180,15 +6162,13 @@
         </is>
       </c>
       <c r="X47" t="n">
-        <v>0.977</v>
+        <v>0.979</v>
       </c>
       <c r="Y47" t="n">
         <v>0</v>
       </c>
-      <c r="Z47" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z47" t="n">
+        <v>1</v>
       </c>
       <c r="AA47" t="n">
         <v>0.974</v>
@@ -6230,7 +6210,7 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>0.891</v>
+        <v>0.892</v>
       </c>
       <c r="G48" t="n">
         <v>0</v>
@@ -6246,7 +6226,7 @@
         <v>78.95</v>
       </c>
       <c r="L48" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M48" t="n">
         <v>0</v>
@@ -6255,7 +6235,7 @@
         <v>78.95</v>
       </c>
       <c r="O48" t="n">
-        <v>0.968</v>
+        <v>0.971</v>
       </c>
       <c r="P48" t="n">
         <v>0</v>
@@ -6266,7 +6246,7 @@
         </is>
       </c>
       <c r="R48" t="n">
-        <v>0.975</v>
+        <v>0.974</v>
       </c>
       <c r="S48" t="n">
         <v>0</v>
@@ -6284,15 +6264,13 @@
         </is>
       </c>
       <c r="X48" t="n">
-        <v>0.978</v>
+        <v>0.981</v>
       </c>
       <c r="Y48" t="n">
         <v>0</v>
       </c>
-      <c r="Z48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z48" t="n">
+        <v>1</v>
       </c>
       <c r="AA48" t="n">
         <v>0.977</v>
@@ -6323,7 +6301,7 @@
         <v>3011295</v>
       </c>
       <c r="C49" t="n">
-        <v>0.975</v>
+        <v>0.974</v>
       </c>
       <c r="D49" t="n">
         <v>0</v>
@@ -6334,7 +6312,7 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>0.896</v>
+        <v>0.895</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
@@ -6359,7 +6337,7 @@
         <v>60.85</v>
       </c>
       <c r="O49" t="n">
-        <v>0.977</v>
+        <v>0.964</v>
       </c>
       <c r="P49" t="n">
         <v>0</v>
@@ -6370,7 +6348,7 @@
         </is>
       </c>
       <c r="R49" t="n">
-        <v>0.976</v>
+        <v>0.979</v>
       </c>
       <c r="S49" t="n">
         <v>0</v>
@@ -6388,18 +6366,16 @@
         </is>
       </c>
       <c r="X49" t="n">
-        <v>0.98</v>
+        <v>0.982</v>
       </c>
       <c r="Y49" t="n">
         <v>0</v>
       </c>
-      <c r="Z49" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z49" t="n">
+        <v>1</v>
       </c>
       <c r="AA49" t="n">
-        <v>0.98</v>
+        <v>0.975</v>
       </c>
       <c r="AB49" t="n">
         <v>0</v>
@@ -6427,7 +6403,7 @@
         <v>4049195</v>
       </c>
       <c r="C50" t="n">
-        <v>0.975</v>
+        <v>0.968</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -6438,7 +6414,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>0.904</v>
+        <v>0.913</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
@@ -6454,7 +6430,7 @@
         <v>34.99</v>
       </c>
       <c r="L50" t="n">
-        <v>0.973</v>
+        <v>0.974</v>
       </c>
       <c r="M50" t="n">
         <v>0</v>
@@ -6463,7 +6439,7 @@
         <v>34.99</v>
       </c>
       <c r="O50" t="n">
-        <v>0.913</v>
+        <v>0.946</v>
       </c>
       <c r="P50" t="n">
         <v>0</v>
@@ -6474,7 +6450,7 @@
         </is>
       </c>
       <c r="R50" t="n">
-        <v>0.962</v>
+        <v>0.9409999999999999</v>
       </c>
       <c r="S50" t="n">
         <v>0</v>
@@ -6492,18 +6468,16 @@
         </is>
       </c>
       <c r="X50" t="n">
+        <v>0.978</v>
+      </c>
+      <c r="Y50" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z50" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA50" t="n">
         <v>0.977</v>
-      </c>
-      <c r="Y50" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z50" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AA50" t="n">
-        <v>0.98</v>
       </c>
       <c r="AB50" t="n">
         <v>0</v>
@@ -6531,7 +6505,7 @@
         <v>4488912</v>
       </c>
       <c r="C51" t="n">
-        <v>0.966</v>
+        <v>0.975</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
@@ -6542,7 +6516,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>0.91</v>
+        <v>0.889</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
@@ -6562,7 +6536,7 @@
         <v>27.95</v>
       </c>
       <c r="L51" t="n">
-        <v>0.972</v>
+        <v>0.968</v>
       </c>
       <c r="M51" t="n">
         <v>0</v>
@@ -6571,7 +6545,7 @@
         <v>27.95</v>
       </c>
       <c r="O51" t="n">
-        <v>0.912</v>
+        <v>0.931</v>
       </c>
       <c r="P51" t="n">
         <v>0</v>
@@ -6582,7 +6556,7 @@
         </is>
       </c>
       <c r="R51" t="n">
-        <v>0.949</v>
+        <v>0.978</v>
       </c>
       <c r="S51" t="n">
         <v>0</v>
@@ -6601,10 +6575,8 @@
       <c r="Y51" t="n">
         <v>0</v>
       </c>
-      <c r="Z51" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z51" t="n">
+        <v>1</v>
       </c>
       <c r="AA51" t="n">
         <v>0.453</v>
@@ -6635,7 +6607,7 @@
         <v>4488912</v>
       </c>
       <c r="C52" t="n">
-        <v>0.971</v>
+        <v>0.972</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -6646,7 +6618,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0.895</v>
+        <v>0.89</v>
       </c>
       <c r="G52" t="n">
         <v>0</v>
@@ -6666,7 +6638,7 @@
         <v>27.95</v>
       </c>
       <c r="L52" t="n">
-        <v>0.975</v>
+        <v>0.976</v>
       </c>
       <c r="M52" t="n">
         <v>0</v>
@@ -6686,7 +6658,7 @@
         </is>
       </c>
       <c r="R52" t="n">
-        <v>0.9409999999999999</v>
+        <v>0.978</v>
       </c>
       <c r="S52" t="n">
         <v>0</v>
@@ -6705,10 +6677,8 @@
       <c r="Y52" t="n">
         <v>0</v>
       </c>
-      <c r="Z52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z52" t="n">
+        <v>1</v>
       </c>
       <c r="AA52" t="n">
         <v>0.453</v>
@@ -6739,7 +6709,7 @@
         <v>7187042</v>
       </c>
       <c r="C53" t="n">
-        <v>0.961</v>
+        <v>0.955</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
@@ -6782,7 +6752,7 @@
         </is>
       </c>
       <c r="R53" t="n">
-        <v>0.9330000000000001</v>
+        <v>0.921</v>
       </c>
       <c r="S53" t="n">
         <v>0</v>
@@ -6800,18 +6770,14 @@
         </is>
       </c>
       <c r="X53" t="n">
+        <v>0.975</v>
+      </c>
+      <c r="Y53" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z53" t="inlineStr"/>
+      <c r="AA53" t="n">
         <v>0.977</v>
-      </c>
-      <c r="Y53" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z53" t="inlineStr">
-        <is>
-          <t>OUT</t>
-        </is>
-      </c>
-      <c r="AA53" t="n">
-        <v>0.976</v>
       </c>
       <c r="AB53" t="n">
         <v>0</v>
@@ -6839,7 +6805,7 @@
         <v>1099589</v>
       </c>
       <c r="C54" t="n">
-        <v>0.949</v>
+        <v>0.951</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -6850,7 +6816,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>0.91</v>
+        <v>0.928</v>
       </c>
       <c r="G54" t="n">
         <v>0</v>
@@ -6866,7 +6832,7 @@
         <v>13.95</v>
       </c>
       <c r="L54" t="n">
-        <v>0.966</v>
+        <v>0.968</v>
       </c>
       <c r="M54" t="n">
         <v>0</v>
@@ -6875,7 +6841,7 @@
         <v>13.95</v>
       </c>
       <c r="O54" t="n">
-        <v>0.896</v>
+        <v>0.913</v>
       </c>
       <c r="P54" t="n">
         <v>0</v>
@@ -6886,7 +6852,7 @@
         </is>
       </c>
       <c r="R54" t="n">
-        <v>0.967</v>
+        <v>0.968</v>
       </c>
       <c r="S54" t="n">
         <v>0</v>
@@ -6904,18 +6870,16 @@
         </is>
       </c>
       <c r="X54" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="Y54" t="n">
         <v>0</v>
       </c>
-      <c r="Z54" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z54" t="n">
+        <v>1</v>
       </c>
       <c r="AA54" t="n">
-        <v>0.973</v>
+        <v>0.974</v>
       </c>
       <c r="AB54" t="n">
         <v>0</v>
@@ -6943,7 +6907,7 @@
         <v>2416691</v>
       </c>
       <c r="C55" t="n">
-        <v>0.951</v>
+        <v>0.961</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -6974,7 +6938,7 @@
         <v>14.95</v>
       </c>
       <c r="L55" t="n">
-        <v>0.968</v>
+        <v>0.973</v>
       </c>
       <c r="M55" t="n">
         <v>0</v>
@@ -6983,7 +6947,7 @@
         <v>29.9</v>
       </c>
       <c r="O55" t="n">
-        <v>0.914</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="P55" t="n">
         <v>0</v>
@@ -6994,7 +6958,7 @@
         </is>
       </c>
       <c r="R55" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.953</v>
       </c>
       <c r="S55" t="n">
         <v>0</v>
@@ -7013,13 +6977,11 @@
       <c r="Y55" t="n">
         <v>0</v>
       </c>
-      <c r="Z55" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z55" t="n">
+        <v>2</v>
       </c>
       <c r="AA55" t="n">
-        <v>0.86</v>
+        <v>0.89</v>
       </c>
       <c r="AB55" t="n">
         <v>0</v>
@@ -7047,7 +7009,7 @@
         <v>2416691</v>
       </c>
       <c r="C56" t="n">
-        <v>0.975</v>
+        <v>0.972</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -7058,7 +7020,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>0.906</v>
+        <v>0.897</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
@@ -7078,7 +7040,7 @@
         <v>14.95</v>
       </c>
       <c r="L56" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M56" t="n">
         <v>0</v>
@@ -7098,7 +7060,7 @@
         </is>
       </c>
       <c r="R56" t="n">
-        <v>0.9419999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="S56" t="n">
         <v>0</v>
@@ -7117,13 +7079,11 @@
       <c r="Y56" t="n">
         <v>0</v>
       </c>
-      <c r="Z56" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z56" t="n">
+        <v>2</v>
       </c>
       <c r="AA56" t="n">
-        <v>0.434</v>
+        <v>0.439</v>
       </c>
       <c r="AB56" t="n">
         <v>0</v>
@@ -7151,7 +7111,7 @@
         <v>6235501</v>
       </c>
       <c r="C57" t="n">
-        <v>0.975</v>
+        <v>0.972</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
@@ -7162,7 +7122,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
@@ -7178,7 +7138,7 @@
         <v>15.99</v>
       </c>
       <c r="L57" t="n">
-        <v>0.976</v>
+        <v>0.978</v>
       </c>
       <c r="M57" t="n">
         <v>0</v>
@@ -7187,7 +7147,7 @@
         <v>15.99</v>
       </c>
       <c r="O57" t="n">
-        <v>0.967</v>
+        <v>0.972</v>
       </c>
       <c r="P57" t="n">
         <v>0</v>
@@ -7198,7 +7158,7 @@
         </is>
       </c>
       <c r="R57" t="n">
-        <v>0.294</v>
+        <v>0.304</v>
       </c>
       <c r="S57" t="n">
         <v>0</v>
@@ -7221,13 +7181,11 @@
       <c r="Y57" t="n">
         <v>0</v>
       </c>
-      <c r="Z57" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z57" t="n">
+        <v>1</v>
       </c>
       <c r="AA57" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
       <c r="AB57" t="n">
         <v>0</v>
@@ -7255,7 +7213,7 @@
         <v>139667</v>
       </c>
       <c r="C58" t="n">
-        <v>0.977</v>
+        <v>0.976</v>
       </c>
       <c r="D58" t="n">
         <v>0</v>
@@ -7266,7 +7224,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>0.821</v>
+        <v>0.822</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
@@ -7295,7 +7253,7 @@
         <v>37.25</v>
       </c>
       <c r="O58" t="n">
-        <v>0.977</v>
+        <v>0.976</v>
       </c>
       <c r="P58" t="n">
         <v>0</v>
@@ -7321,10 +7279,8 @@
       <c r="Y58" t="n">
         <v>0</v>
       </c>
-      <c r="Z58" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="Z58" t="n">
+        <v>5</v>
       </c>
       <c r="AA58" t="n">
         <v>0.058</v>
@@ -7355,7 +7311,7 @@
         <v>2441285</v>
       </c>
       <c r="C59" t="n">
-        <v>0.977</v>
+        <v>0.974</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -7366,7 +7322,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>0.896</v>
+        <v>0.895</v>
       </c>
       <c r="G59" t="n">
         <v>0</v>
@@ -7382,7 +7338,7 @@
         <v>10.99</v>
       </c>
       <c r="L59" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M59" t="n">
         <v>0</v>
@@ -7402,7 +7358,7 @@
         </is>
       </c>
       <c r="R59" t="n">
-        <v>0.961</v>
+        <v>0.973</v>
       </c>
       <c r="S59" t="n">
         <v>0</v>
@@ -7420,18 +7376,16 @@
         </is>
       </c>
       <c r="X59" t="n">
-        <v>0.982</v>
+        <v>0.983</v>
       </c>
       <c r="Y59" t="n">
         <v>0</v>
       </c>
-      <c r="Z59" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z59" t="n">
+        <v>2</v>
       </c>
       <c r="AA59" t="n">
-        <v>0.981</v>
+        <v>0.983</v>
       </c>
       <c r="AB59" t="n">
         <v>0</v>
@@ -7459,7 +7413,7 @@
         <v>7000181</v>
       </c>
       <c r="C60" t="n">
-        <v>0.976</v>
+        <v>0.974</v>
       </c>
       <c r="D60" t="n">
         <v>0</v>
@@ -7470,7 +7424,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0.885</v>
+        <v>0.852</v>
       </c>
       <c r="G60" t="n">
         <v>0</v>
@@ -7486,7 +7440,7 @@
         <v>56.99</v>
       </c>
       <c r="L60" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M60" t="n">
         <v>0</v>
@@ -7495,7 +7449,7 @@
         <v>113.98</v>
       </c>
       <c r="O60" t="n">
-        <v>0.973</v>
+        <v>0.969</v>
       </c>
       <c r="P60" t="n">
         <v>0</v>
@@ -7506,7 +7460,7 @@
         </is>
       </c>
       <c r="R60" t="n">
-        <v>0.968</v>
+        <v>0.966</v>
       </c>
       <c r="S60" t="n">
         <v>0</v>
@@ -7524,15 +7478,13 @@
         </is>
       </c>
       <c r="X60" t="n">
-        <v>0.977</v>
+        <v>0.979</v>
       </c>
       <c r="Y60" t="n">
         <v>0</v>
       </c>
-      <c r="Z60" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z60" t="n">
+        <v>2</v>
       </c>
       <c r="AA60" t="n">
         <v>0.978</v>
@@ -7563,7 +7515,7 @@
         <v>4421109</v>
       </c>
       <c r="C61" t="n">
-        <v>0.975</v>
+        <v>0.973</v>
       </c>
       <c r="D61" t="n">
         <v>0</v>
@@ -7574,7 +7526,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.851</v>
+        <v>0.852</v>
       </c>
       <c r="G61" t="n">
         <v>0</v>
@@ -7599,7 +7551,7 @@
         <v>87.95</v>
       </c>
       <c r="O61" t="n">
-        <v>0.973</v>
+        <v>0.97</v>
       </c>
       <c r="P61" t="n">
         <v>0</v>
@@ -7610,7 +7562,7 @@
         </is>
       </c>
       <c r="R61" t="n">
-        <v>0.977</v>
+        <v>0.971</v>
       </c>
       <c r="S61" t="n">
         <v>0</v>
@@ -7628,18 +7580,16 @@
         </is>
       </c>
       <c r="X61" t="n">
-        <v>0.978</v>
+        <v>0.98</v>
       </c>
       <c r="Y61" t="n">
         <v>0</v>
       </c>
-      <c r="Z61" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z61" t="n">
+        <v>1</v>
       </c>
       <c r="AA61" t="n">
-        <v>0.976</v>
+        <v>0.975</v>
       </c>
       <c r="AB61" t="n">
         <v>0</v>
@@ -7694,7 +7644,7 @@
         <v>79.59</v>
       </c>
       <c r="L62" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M62" t="n">
         <v>0</v>
@@ -7703,7 +7653,7 @@
         <v>79.59</v>
       </c>
       <c r="O62" t="n">
-        <v>0.975</v>
+        <v>0.972</v>
       </c>
       <c r="P62" t="n">
         <v>0</v>
@@ -7714,7 +7664,7 @@
         </is>
       </c>
       <c r="R62" t="n">
-        <v>0.291</v>
+        <v>0.294</v>
       </c>
       <c r="S62" t="n">
         <v>0</v>
@@ -7737,10 +7687,8 @@
       <c r="Y62" t="n">
         <v>0</v>
       </c>
-      <c r="Z62" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z62" t="n">
+        <v>1</v>
       </c>
       <c r="AA62" t="n">
         <v>0.977</v>
@@ -7771,7 +7719,7 @@
         <v>5625660</v>
       </c>
       <c r="C63" t="n">
-        <v>0.967</v>
+        <v>0.973</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
@@ -7782,7 +7730,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>0.825</v>
+        <v>0.819</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
@@ -7802,7 +7750,7 @@
         <v>37.95</v>
       </c>
       <c r="L63" t="n">
-        <v>0.974</v>
+        <v>0.975</v>
       </c>
       <c r="M63" t="n">
         <v>0</v>
@@ -7811,7 +7759,7 @@
         <v>75.90000000000001</v>
       </c>
       <c r="O63" t="n">
-        <v>0.947</v>
+        <v>0.953</v>
       </c>
       <c r="P63" t="n">
         <v>0</v>
@@ -7822,7 +7770,7 @@
         </is>
       </c>
       <c r="R63" t="n">
-        <v>0.966</v>
+        <v>0.974</v>
       </c>
       <c r="S63" t="n">
         <v>0</v>
@@ -7841,10 +7789,8 @@
       <c r="Y63" t="n">
         <v>0</v>
       </c>
-      <c r="Z63" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z63" t="n">
+        <v>2</v>
       </c>
       <c r="AA63" t="n">
         <v>0.058</v>
@@ -7875,7 +7821,7 @@
         <v>6404743</v>
       </c>
       <c r="C64" t="n">
-        <v>0.976</v>
+        <v>0.973</v>
       </c>
       <c r="D64" t="n">
         <v>0</v>
@@ -7886,7 +7832,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>0.891</v>
+        <v>0.854</v>
       </c>
       <c r="G64" t="n">
         <v>0</v>
@@ -7906,7 +7852,7 @@
         <v>31.95</v>
       </c>
       <c r="L64" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M64" t="n">
         <v>0</v>
@@ -7915,7 +7861,7 @@
         <v>31.95</v>
       </c>
       <c r="O64" t="n">
-        <v>0.977</v>
+        <v>0.972</v>
       </c>
       <c r="P64" t="n">
         <v>0</v>
@@ -7926,7 +7872,7 @@
         </is>
       </c>
       <c r="R64" t="n">
-        <v>0.947</v>
+        <v>0.962</v>
       </c>
       <c r="S64" t="n">
         <v>0</v>
@@ -7945,10 +7891,8 @@
       <c r="Y64" t="n">
         <v>0</v>
       </c>
-      <c r="Z64" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z64" t="n">
+        <v>1</v>
       </c>
       <c r="AA64" t="n">
         <v>0.058</v>
@@ -7979,7 +7923,7 @@
         <v>7762299</v>
       </c>
       <c r="C65" t="n">
-        <v>0.976</v>
+        <v>0.973</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
@@ -7990,7 +7934,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>0.897</v>
+        <v>0.896</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
@@ -8010,7 +7954,7 @@
         <v>27.95</v>
       </c>
       <c r="L65" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M65" t="n">
         <v>0</v>
@@ -8019,7 +7963,7 @@
         <v>27.95</v>
       </c>
       <c r="O65" t="n">
-        <v>0.974</v>
+        <v>0.967</v>
       </c>
       <c r="P65" t="n">
         <v>0</v>
@@ -8044,18 +7988,16 @@
         </is>
       </c>
       <c r="X65" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="Y65" t="n">
         <v>0</v>
       </c>
-      <c r="Z65" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z65" t="n">
+        <v>1</v>
       </c>
       <c r="AA65" t="n">
-        <v>0.978</v>
+        <v>0.977</v>
       </c>
       <c r="AB65" t="n">
         <v>0</v>
@@ -8083,7 +8025,7 @@
         <v>9793688</v>
       </c>
       <c r="C66" t="n">
-        <v>0.975</v>
+        <v>0.973</v>
       </c>
       <c r="D66" t="n">
         <v>0</v>
@@ -8094,7 +8036,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>0.799</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="G66" t="n">
         <v>0</v>
@@ -8110,7 +8052,7 @@
         <v>144.29</v>
       </c>
       <c r="L66" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="M66" t="n">
         <v>0</v>
@@ -8119,18 +8061,18 @@
         <v>144.29</v>
       </c>
       <c r="O66" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="P66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>65LB</t>
+        </is>
+      </c>
+      <c r="R66" t="n">
         <v>0.974</v>
-      </c>
-      <c r="P66" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>65LB</t>
-        </is>
-      </c>
-      <c r="R66" t="n">
-        <v>0.969</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -8153,10 +8095,8 @@
       <c r="Y66" t="n">
         <v>0</v>
       </c>
-      <c r="Z66" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z66" t="n">
+        <v>1</v>
       </c>
       <c r="AA66" t="n">
         <v>0.976</v>
@@ -8187,7 +8127,7 @@
         <v>952018</v>
       </c>
       <c r="C67" t="n">
-        <v>0.973</v>
+        <v>0.974</v>
       </c>
       <c r="D67" t="n">
         <v>0</v>
@@ -8198,7 +8138,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>0.868</v>
+        <v>0.886</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
@@ -8214,7 +8154,7 @@
         <v>49.25</v>
       </c>
       <c r="L67" t="n">
-        <v>0.976</v>
+        <v>0.977</v>
       </c>
       <c r="M67" t="n">
         <v>0</v>
@@ -8223,18 +8163,18 @@
         <v>49.25</v>
       </c>
       <c r="O67" t="n">
+        <v>0.973</v>
+      </c>
+      <c r="P67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>10100</t>
+        </is>
+      </c>
+      <c r="R67" t="n">
         <v>0.975</v>
-      </c>
-      <c r="P67" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>10100</t>
-        </is>
-      </c>
-      <c r="R67" t="n">
-        <v>0.972</v>
       </c>
       <c r="S67" t="n">
         <v>0</v>
@@ -8252,18 +8192,16 @@
         </is>
       </c>
       <c r="X67" t="n">
-        <v>0.982</v>
+        <v>0.981</v>
       </c>
       <c r="Y67" t="n">
         <v>0</v>
       </c>
-      <c r="Z67" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z67" t="n">
+        <v>1</v>
       </c>
       <c r="AA67" t="n">
-        <v>0.986</v>
+        <v>0.981</v>
       </c>
       <c r="AB67" t="n">
         <v>0</v>
@@ -8291,7 +8229,7 @@
         <v>5482575</v>
       </c>
       <c r="C68" t="n">
-        <v>0.971</v>
+        <v>0.972</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
@@ -8302,7 +8240,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>0.614</v>
+        <v>0.643</v>
       </c>
       <c r="G68" t="n">
         <v>0</v>
@@ -8318,7 +8256,7 @@
         <v>76.34999999999999</v>
       </c>
       <c r="L68" t="n">
-        <v>0.976</v>
+        <v>0.977</v>
       </c>
       <c r="M68" t="n">
         <v>0</v>
@@ -8327,7 +8265,7 @@
         <v>76.34999999999999</v>
       </c>
       <c r="O68" t="n">
-        <v>0.961</v>
+        <v>0.967</v>
       </c>
       <c r="P68" t="n">
         <v>0</v>
@@ -8352,18 +8290,16 @@
         </is>
       </c>
       <c r="X68" t="n">
-        <v>0.98</v>
+        <v>0.979</v>
       </c>
       <c r="Y68" t="n">
         <v>0</v>
       </c>
-      <c r="Z68" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z68" t="n">
+        <v>1</v>
       </c>
       <c r="AA68" t="n">
-        <v>0.977</v>
+        <v>0.974</v>
       </c>
       <c r="AB68" t="n">
         <v>0</v>
@@ -8391,7 +8327,7 @@
         <v>8003370</v>
       </c>
       <c r="C69" t="n">
-        <v>0.969</v>
+        <v>0.968</v>
       </c>
       <c r="D69" t="n">
         <v>0</v>
@@ -8418,7 +8354,7 @@
         <v>52.99</v>
       </c>
       <c r="L69" t="n">
-        <v>0.976</v>
+        <v>0.977</v>
       </c>
       <c r="M69" t="n">
         <v>0</v>
@@ -8427,7 +8363,7 @@
         <v>105.98</v>
       </c>
       <c r="O69" t="n">
-        <v>0.967</v>
+        <v>0.969</v>
       </c>
       <c r="P69" t="n">
         <v>0</v>
@@ -8457,13 +8393,11 @@
       <c r="Y69" t="n">
         <v>0</v>
       </c>
-      <c r="Z69" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z69" t="n">
+        <v>2</v>
       </c>
       <c r="AA69" t="n">
-        <v>0.977</v>
+        <v>0.976</v>
       </c>
       <c r="AB69" t="n">
         <v>0</v>
@@ -8502,7 +8436,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>0.273</v>
+        <v>0.272</v>
       </c>
       <c r="G70" t="n">
         <v>0</v>
@@ -8527,7 +8461,7 @@
         <v>105.9</v>
       </c>
       <c r="O70" t="n">
-        <v>0.164</v>
+        <v>0.162</v>
       </c>
       <c r="P70" t="n">
         <v>0</v>
@@ -8538,7 +8472,7 @@
         </is>
       </c>
       <c r="R70" t="n">
-        <v>0.906</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="S70" t="n">
         <v>0</v>
@@ -8561,13 +8495,11 @@
       <c r="Y70" t="n">
         <v>0</v>
       </c>
-      <c r="Z70" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z70" t="n">
+        <v>2</v>
       </c>
       <c r="AA70" t="n">
-        <v>0.977</v>
+        <v>0.976</v>
       </c>
       <c r="AB70" t="n">
         <v>0</v>
@@ -8625,10 +8557,8 @@
       <c r="W71" t="inlineStr"/>
       <c r="X71" t="inlineStr"/>
       <c r="Y71" t="inlineStr"/>
-      <c r="Z71" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z71" t="n">
+        <v>1</v>
       </c>
       <c r="AA71" t="inlineStr"/>
       <c r="AB71" t="inlineStr"/>
@@ -8647,7 +8577,7 @@
         <v>7101689</v>
       </c>
       <c r="C72" t="n">
-        <v>0.976</v>
+        <v>0.975</v>
       </c>
       <c r="D72" t="n">
         <v>0</v>
@@ -8658,7 +8588,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>0.949</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G72" t="n">
         <v>0</v>
@@ -8674,7 +8604,7 @@
         <v>39.39</v>
       </c>
       <c r="L72" t="n">
-        <v>0.977</v>
+        <v>0.98</v>
       </c>
       <c r="M72" t="n">
         <v>0</v>
@@ -8683,7 +8613,7 @@
         <v>39.39</v>
       </c>
       <c r="O72" t="n">
-        <v>0.972</v>
+        <v>0.974</v>
       </c>
       <c r="P72" t="n">
         <v>0</v>
@@ -8694,7 +8624,7 @@
         </is>
       </c>
       <c r="R72" t="n">
-        <v>0.964</v>
+        <v>0.969</v>
       </c>
       <c r="S72" t="n">
         <v>0</v>
@@ -8712,18 +8642,16 @@
         </is>
       </c>
       <c r="X72" t="n">
-        <v>0.978</v>
+        <v>0.983</v>
       </c>
       <c r="Y72" t="n">
         <v>0</v>
       </c>
-      <c r="Z72" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z72" t="n">
+        <v>1</v>
       </c>
       <c r="AA72" t="n">
-        <v>0.977</v>
+        <v>0.982</v>
       </c>
       <c r="AB72" t="n">
         <v>0</v>
@@ -8744,10 +8672,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A73" t="n">
+        <v>652144509</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -8755,7 +8681,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.98</v>
+        <v>0.979</v>
       </c>
       <c r="D73" t="n">
         <v>0</v>
@@ -8786,7 +8712,7 @@
         <v>7.39</v>
       </c>
       <c r="L73" t="n">
-        <v>0.981</v>
+        <v>0.982</v>
       </c>
       <c r="M73" t="n">
         <v>0</v>
@@ -8795,7 +8721,7 @@
         <v>14.78</v>
       </c>
       <c r="O73" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="P73" t="n">
         <v>0</v>
@@ -8806,7 +8732,7 @@
         </is>
       </c>
       <c r="R73" t="n">
-        <v>0.506</v>
+        <v>0.522</v>
       </c>
       <c r="S73" t="n">
         <v>0</v>
@@ -8825,10 +8751,8 @@
       <c r="Y73" t="n">
         <v>0</v>
       </c>
-      <c r="Z73" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z73" t="n">
+        <v>2</v>
       </c>
       <c r="AA73" t="n">
         <v>0.528</v>
@@ -8852,10 +8776,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A74" t="n">
+        <v>652144509</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -8863,7 +8785,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.982</v>
+        <v>0.98</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
@@ -8874,7 +8796,7 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>0.804</v>
+        <v>0.799</v>
       </c>
       <c r="G74" t="n">
         <v>0</v>
@@ -8894,7 +8816,7 @@
         <v>21.99</v>
       </c>
       <c r="L74" t="n">
-        <v>0.982</v>
+        <v>0.986</v>
       </c>
       <c r="M74" t="n">
         <v>0</v>
@@ -8903,7 +8825,7 @@
         <v>21.99</v>
       </c>
       <c r="O74" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="P74" t="n">
         <v>0</v>
@@ -8914,7 +8836,7 @@
         </is>
       </c>
       <c r="R74" t="n">
-        <v>0.975</v>
+        <v>0.982</v>
       </c>
       <c r="S74" t="n">
         <v>0</v>
@@ -8933,10 +8855,8 @@
       <c r="Y74" t="n">
         <v>0</v>
       </c>
-      <c r="Z74" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z74" t="n">
+        <v>1</v>
       </c>
       <c r="AA74" t="n">
         <v>0.528</v>
@@ -8960,10 +8880,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A75" t="n">
+        <v>652144509</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -8971,7 +8889,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.98</v>
+        <v>0.978</v>
       </c>
       <c r="D75" t="n">
         <v>0</v>
@@ -8982,7 +8900,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>0.822</v>
+        <v>0.823</v>
       </c>
       <c r="G75" t="n">
         <v>0</v>
@@ -8998,7 +8916,7 @@
         <v>10.99</v>
       </c>
       <c r="L75" t="n">
-        <v>0.983</v>
+        <v>0.982</v>
       </c>
       <c r="M75" t="n">
         <v>0</v>
@@ -9007,7 +8925,7 @@
         <v>21.98</v>
       </c>
       <c r="O75" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="P75" t="n">
         <v>0</v>
@@ -9018,7 +8936,7 @@
         </is>
       </c>
       <c r="R75" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="S75" t="n">
         <v>0</v>
@@ -9041,13 +8959,11 @@
       <c r="Y75" t="n">
         <v>0</v>
       </c>
-      <c r="Z75" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="Z75" t="n">
+        <v>2</v>
       </c>
       <c r="AA75" t="n">
-        <v>0.984</v>
+        <v>0.986</v>
       </c>
       <c r="AB75" t="n">
         <v>0</v>
@@ -9068,10 +8984,8 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A76" t="n">
+        <v>652144509</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -9079,7 +8993,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.98</v>
+        <v>0.978</v>
       </c>
       <c r="D76" t="n">
         <v>0</v>
@@ -9090,7 +9004,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0.822</v>
+        <v>0.819</v>
       </c>
       <c r="G76" t="n">
         <v>0</v>
@@ -9106,7 +9020,7 @@
         <v>80.98999999999999</v>
       </c>
       <c r="L76" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="M76" t="n">
         <v>0</v>
@@ -9115,7 +9029,7 @@
         <v>80.98999999999999</v>
       </c>
       <c r="O76" t="n">
-        <v>0.975</v>
+        <v>0.977</v>
       </c>
       <c r="P76" t="n">
         <v>0</v>
@@ -9126,7 +9040,7 @@
         </is>
       </c>
       <c r="R76" t="n">
-        <v>0.961</v>
+        <v>0.969</v>
       </c>
       <c r="S76" t="n">
         <v>0</v>
@@ -9149,13 +9063,11 @@
       <c r="Y76" t="n">
         <v>0</v>
       </c>
-      <c r="Z76" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z76" t="n">
+        <v>1</v>
       </c>
       <c r="AA76" t="n">
-        <v>0.982</v>
+        <v>0.984</v>
       </c>
       <c r="AB76" t="n">
         <v>0</v>
@@ -9176,10 +9088,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A77" t="n">
+        <v>652144509</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -9187,7 +9097,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0.979</v>
+        <v>0.978</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
@@ -9198,7 +9108,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>0.84</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="G77" t="n">
         <v>0</v>
@@ -9214,7 +9124,7 @@
         <v>111.95</v>
       </c>
       <c r="L77" t="n">
-        <v>0.98</v>
+        <v>0.981</v>
       </c>
       <c r="M77" t="n">
         <v>0</v>
@@ -9223,7 +9133,7 @@
         <v>111.95</v>
       </c>
       <c r="O77" t="n">
-        <v>0.975</v>
+        <v>0.976</v>
       </c>
       <c r="P77" t="n">
         <v>0</v>
@@ -9234,7 +9144,7 @@
         </is>
       </c>
       <c r="R77" t="n">
-        <v>0.961</v>
+        <v>0.962</v>
       </c>
       <c r="S77" t="n">
         <v>0</v>
@@ -9257,10 +9167,8 @@
       <c r="Y77" t="n">
         <v>0</v>
       </c>
-      <c r="Z77" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z77" t="n">
+        <v>1</v>
       </c>
       <c r="AA77" t="n">
         <v>0.977</v>
@@ -9284,10 +9192,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A78" t="n">
+        <v>652144509</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -9295,7 +9201,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.978</v>
+        <v>0.977</v>
       </c>
       <c r="D78" t="n">
         <v>0</v>
@@ -9306,7 +9212,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>0.821</v>
+        <v>0.822</v>
       </c>
       <c r="G78" t="n">
         <v>0</v>
@@ -9331,7 +9237,7 @@
         <v>54.95</v>
       </c>
       <c r="O78" t="n">
-        <v>0.977</v>
+        <v>0.974</v>
       </c>
       <c r="P78" t="n">
         <v>0</v>
@@ -9360,18 +9266,16 @@
         </is>
       </c>
       <c r="X78" t="n">
-        <v>0.982</v>
+        <v>0.985</v>
       </c>
       <c r="Y78" t="n">
         <v>0</v>
       </c>
-      <c r="Z78" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z78" t="n">
+        <v>1</v>
       </c>
       <c r="AA78" t="n">
-        <v>0.978</v>
+        <v>0.977</v>
       </c>
       <c r="AB78" t="n">
         <v>0</v>
@@ -9392,10 +9296,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A79" t="n">
+        <v>652144509</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -9468,18 +9370,16 @@
         </is>
       </c>
       <c r="X79" t="n">
-        <v>0.983</v>
+        <v>0.986</v>
       </c>
       <c r="Y79" t="n">
         <v>0</v>
       </c>
-      <c r="Z79" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z79" t="n">
+        <v>1</v>
       </c>
       <c r="AA79" t="n">
-        <v>0.98</v>
+        <v>0.979</v>
       </c>
       <c r="AB79" t="n">
         <v>0</v>
@@ -9500,10 +9400,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A80" t="n">
+        <v>652144509</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -9522,7 +9420,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>0.744</v>
+        <v>0.751</v>
       </c>
       <c r="G80" t="n">
         <v>0</v>
@@ -9542,7 +9440,7 @@
         <v>72.45</v>
       </c>
       <c r="L80" t="n">
-        <v>0.979</v>
+        <v>0.985</v>
       </c>
       <c r="M80" t="n">
         <v>0</v>
@@ -9551,7 +9449,7 @@
         <v>72.45</v>
       </c>
       <c r="O80" t="n">
-        <v>0.977</v>
+        <v>0.98</v>
       </c>
       <c r="P80" t="n">
         <v>0</v>
@@ -9576,18 +9474,16 @@
         </is>
       </c>
       <c r="X80" t="n">
-        <v>0.983</v>
+        <v>0.986</v>
       </c>
       <c r="Y80" t="n">
         <v>0</v>
       </c>
-      <c r="Z80" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z80" t="n">
+        <v>1</v>
       </c>
       <c r="AA80" t="n">
-        <v>0.98</v>
+        <v>0.977</v>
       </c>
       <c r="AB80" t="n">
         <v>0</v>
@@ -9608,10 +9504,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A81" t="n">
+        <v>652144509</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -9630,7 +9524,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>0.745</v>
+        <v>0.74</v>
       </c>
       <c r="G81" t="n">
         <v>0</v>
@@ -9655,7 +9549,7 @@
         <v>60.85</v>
       </c>
       <c r="O81" t="n">
-        <v>0.982</v>
+        <v>0.977</v>
       </c>
       <c r="P81" t="n">
         <v>0</v>
@@ -9666,7 +9560,7 @@
         </is>
       </c>
       <c r="R81" t="n">
-        <v>0.978</v>
+        <v>0.983</v>
       </c>
       <c r="S81" t="n">
         <v>0</v>
@@ -9689,13 +9583,11 @@
       <c r="Y81" t="n">
         <v>0</v>
       </c>
-      <c r="Z81" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z81" t="n">
+        <v>1</v>
       </c>
       <c r="AA81" t="n">
-        <v>0.979</v>
+        <v>0.977</v>
       </c>
       <c r="AB81" t="n">
         <v>0</v>
@@ -9716,10 +9608,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A82" t="n">
+        <v>652144509</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -9727,7 +9617,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="D82" t="n">
         <v>0</v>
@@ -9738,7 +9628,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>0.677</v>
+        <v>0.739</v>
       </c>
       <c r="G82" t="n">
         <v>0</v>
@@ -9758,7 +9648,7 @@
         <v>27.95</v>
       </c>
       <c r="L82" t="n">
-        <v>0.979</v>
+        <v>0.98</v>
       </c>
       <c r="M82" t="n">
         <v>0</v>
@@ -9767,7 +9657,7 @@
         <v>27.95</v>
       </c>
       <c r="O82" t="n">
-        <v>0.978</v>
+        <v>0.977</v>
       </c>
       <c r="P82" t="n">
         <v>0</v>
@@ -9778,7 +9668,7 @@
         </is>
       </c>
       <c r="R82" t="n">
-        <v>0.975</v>
+        <v>0.981</v>
       </c>
       <c r="S82" t="n">
         <v>0</v>
@@ -9797,10 +9687,8 @@
       <c r="Y82" t="n">
         <v>0</v>
       </c>
-      <c r="Z82" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z82" t="n">
+        <v>1</v>
       </c>
       <c r="AA82" t="n">
         <v>0.528</v>
@@ -9824,10 +9712,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A83" t="n">
+        <v>652144509</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -9835,7 +9721,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.98</v>
+        <v>0.978</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
@@ -9846,7 +9732,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>0.863</v>
+        <v>0.864</v>
       </c>
       <c r="G83" t="n">
         <v>0</v>
@@ -9862,7 +9748,7 @@
         <v>89.95</v>
       </c>
       <c r="L83" t="n">
-        <v>0.981</v>
+        <v>0.982</v>
       </c>
       <c r="M83" t="n">
         <v>0</v>
@@ -9882,7 +9768,7 @@
         </is>
       </c>
       <c r="R83" t="n">
-        <v>0.951</v>
+        <v>0.961</v>
       </c>
       <c r="S83" t="n">
         <v>0</v>
@@ -9905,13 +9791,11 @@
       <c r="Y83" t="n">
         <v>0</v>
       </c>
-      <c r="Z83" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z83" t="n">
+        <v>1</v>
       </c>
       <c r="AA83" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="AB83" t="n">
         <v>0</v>
@@ -9932,10 +9816,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A84" t="n">
+        <v>652144509</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -9943,7 +9825,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0.979</v>
+        <v>0.981</v>
       </c>
       <c r="D84" t="n">
         <v>0</v>
@@ -9954,7 +9836,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>0.87</v>
+        <v>0.853</v>
       </c>
       <c r="G84" t="n">
         <v>0</v>
@@ -9970,7 +9852,7 @@
         <v>49.25</v>
       </c>
       <c r="L84" t="n">
-        <v>0.983</v>
+        <v>0.981</v>
       </c>
       <c r="M84" t="n">
         <v>0</v>
@@ -9990,7 +9872,7 @@
         </is>
       </c>
       <c r="R84" t="n">
-        <v>0.978</v>
+        <v>0.979</v>
       </c>
       <c r="S84" t="n">
         <v>0</v>
@@ -10008,18 +9890,16 @@
         </is>
       </c>
       <c r="X84" t="n">
-        <v>0.987</v>
+        <v>0.986</v>
       </c>
       <c r="Y84" t="n">
         <v>0</v>
       </c>
-      <c r="Z84" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z84" t="n">
+        <v>1</v>
       </c>
       <c r="AA84" t="n">
-        <v>0.986</v>
+        <v>0.985</v>
       </c>
       <c r="AB84" t="n">
         <v>0</v>
@@ -10040,10 +9920,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>652144509</t>
-        </is>
+      <c r="A85" t="n">
+        <v>652144509</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -10051,7 +9929,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0.98</v>
+        <v>0.979</v>
       </c>
       <c r="D85" t="n">
         <v>0</v>
@@ -10062,7 +9940,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>0.822</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="G85" t="n">
         <v>0</v>
@@ -10082,7 +9960,7 @@
         <v>14.95</v>
       </c>
       <c r="L85" t="n">
-        <v>0.982</v>
+        <v>0.984</v>
       </c>
       <c r="M85" t="n">
         <v>0</v>
@@ -10091,7 +9969,7 @@
         <v>14.95</v>
       </c>
       <c r="O85" t="n">
-        <v>0.977</v>
+        <v>0.978</v>
       </c>
       <c r="P85" t="n">
         <v>0</v>
@@ -10102,7 +9980,7 @@
         </is>
       </c>
       <c r="R85" t="n">
-        <v>0.975</v>
+        <v>0.978</v>
       </c>
       <c r="S85" t="n">
         <v>0</v>
@@ -10121,13 +9999,11 @@
       <c r="Y85" t="n">
         <v>0</v>
       </c>
-      <c r="Z85" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="Z85" t="n">
+        <v>1</v>
       </c>
       <c r="AA85" t="n">
-        <v>0.974</v>
+        <v>0.976</v>
       </c>
       <c r="AB85" t="n">
         <v>0</v>

</xml_diff>